<commit_message>
put Mikefile.idf in gitignore
</commit_message>
<xml_diff>
--- a/data/all-variables-exp3.xlsx
+++ b/data/all-variables-exp3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikewood/Dropbox/COLBE/Git-cntl-weather-file-analysis/Weather file analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike-wood\Dropbox\COLBE\Git-cntl-weather-file-analysis\Weather file analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>p1</t>
   </si>
@@ -282,12 +282,15 @@
   </si>
   <si>
     <t>Alfonso (type of building)</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -650,13 +653,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -727,10 +730,13 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -744,10 +750,13 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,7 +1000,10 @@
         <v>0.3</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1008,7 +1020,10 @@
         <v>0.3</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1025,7 +1040,10 @@
         <v>0.3</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1042,7 +1060,10 @@
         <v>0.3</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>